<commit_message>
Modify the displayed state value of the button.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="53">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -165,6 +165,15 @@
   </si>
   <si>
     <t xml:space="preserve">32-126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button0</t>
   </si>
 </sst>
 </file>
@@ -1662,7 +1671,7 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>